<commit_message>
removed a duplicate column
</commit_message>
<xml_diff>
--- a/dataset_complete.xlsx
+++ b/dataset_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2204\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AB56309-EBD2-4C03-B5D5-67C3AE471949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A504866-7D74-4F54-9A50-1ED1B46D38B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="213">
   <si>
     <t>car_ID</t>
   </si>
@@ -1519,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE206"/>
+  <dimension ref="A1:AD206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q186" workbookViewId="0">
-      <selection activeCell="AD207" sqref="AD207"/>
+    <sheetView tabSelected="1" topLeftCell="V106" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1533,7 +1533,7 @@
     <col min="31" max="31" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1624,11 +1624,8 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1719,11 +1716,8 @@
       <c r="AD2">
         <v>18252</v>
       </c>
-      <c r="AE2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1814,11 +1808,8 @@
       <c r="AD3">
         <v>10539</v>
       </c>
-      <c r="AE3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1909,11 +1900,8 @@
       <c r="AD4">
         <v>6297</v>
       </c>
-      <c r="AE4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2004,11 +1992,8 @@
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2099,11 +2084,8 @@
       <c r="AD6">
         <v>0</v>
       </c>
-      <c r="AE6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2194,11 +2176,8 @@
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31">
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2289,11 +2268,8 @@
       <c r="AD8">
         <v>0</v>
       </c>
-      <c r="AE8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31">
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2384,11 +2360,8 @@
       <c r="AD9">
         <v>0</v>
       </c>
-      <c r="AE9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31">
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2479,11 +2452,8 @@
       <c r="AD10">
         <v>0</v>
       </c>
-      <c r="AE10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2574,11 +2544,8 @@
       <c r="AD11">
         <v>0</v>
       </c>
-      <c r="AE11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31">
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2669,11 +2636,8 @@
       <c r="AD12">
         <v>113209</v>
       </c>
-      <c r="AE12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2764,11 +2728,8 @@
       <c r="AD13">
         <v>113209</v>
       </c>
-      <c r="AE13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2859,11 +2820,8 @@
       <c r="AD14">
         <v>86749</v>
       </c>
-      <c r="AE14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2954,11 +2912,8 @@
       <c r="AD15">
         <v>81466</v>
       </c>
-      <c r="AE15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3049,11 +3004,8 @@
       <c r="AD16">
         <v>7571</v>
       </c>
-      <c r="AE16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31">
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3144,11 +3096,8 @@
       <c r="AD17">
         <v>15151</v>
       </c>
-      <c r="AE17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31">
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3239,11 +3188,8 @@
       <c r="AD18">
         <v>43103</v>
       </c>
-      <c r="AE18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31">
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3334,11 +3280,8 @@
       <c r="AD19">
         <v>81466</v>
       </c>
-      <c r="AE19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31">
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3429,11 +3372,8 @@
       <c r="AD20">
         <v>750</v>
       </c>
-      <c r="AE20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31">
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3524,11 +3464,8 @@
       <c r="AD21">
         <v>0</v>
       </c>
-      <c r="AE21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31">
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3619,11 +3556,8 @@
       <c r="AD22">
         <v>0</v>
       </c>
-      <c r="AE22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31">
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3714,11 +3648,8 @@
       <c r="AD23">
         <v>0</v>
       </c>
-      <c r="AE23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31">
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3809,11 +3740,8 @@
       <c r="AD24">
         <v>54314</v>
       </c>
-      <c r="AE24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31">
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3904,11 +3832,8 @@
       <c r="AD25">
         <v>0</v>
       </c>
-      <c r="AE25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31">
+    </row>
+    <row r="26" spans="1:30">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3999,11 +3924,8 @@
       <c r="AD26">
         <v>0</v>
       </c>
-      <c r="AE26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31">
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4094,11 +4016,8 @@
       <c r="AD27">
         <v>0</v>
       </c>
-      <c r="AE27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31">
+    </row>
+    <row r="28" spans="1:30">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4189,11 +4108,8 @@
       <c r="AD28">
         <v>0</v>
       </c>
-      <c r="AE28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31">
+    </row>
+    <row r="29" spans="1:30">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4284,11 +4200,8 @@
       <c r="AD29">
         <v>0</v>
       </c>
-      <c r="AE29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31">
+    </row>
+    <row r="30" spans="1:30">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4379,11 +4292,8 @@
       <c r="AD30">
         <v>10</v>
       </c>
-      <c r="AE30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31">
+    </row>
+    <row r="31" spans="1:30">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4474,11 +4384,8 @@
       <c r="AD31">
         <v>0</v>
       </c>
-      <c r="AE31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31">
+    </row>
+    <row r="32" spans="1:30">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4569,11 +4476,8 @@
       <c r="AD32">
         <v>263767</v>
       </c>
-      <c r="AE32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31">
+    </row>
+    <row r="33" spans="1:30">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4652,11 +4556,8 @@
       <c r="Z33">
         <v>6855</v>
       </c>
-      <c r="AE33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31">
+    </row>
+    <row r="34" spans="1:30">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4735,11 +4636,8 @@
       <c r="Z34">
         <v>5399</v>
       </c>
-      <c r="AE34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31">
+    </row>
+    <row r="35" spans="1:30">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4830,11 +4728,8 @@
       <c r="AD35">
         <v>0</v>
       </c>
-      <c r="AE35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31">
+    </row>
+    <row r="36" spans="1:30">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4913,11 +4808,8 @@
       <c r="Z36">
         <v>7129</v>
       </c>
-      <c r="AE36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" ht="15.75">
+    </row>
+    <row r="37" spans="1:30" ht="15.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5008,11 +4900,8 @@
       <c r="AD37">
         <v>202676</v>
       </c>
-      <c r="AE37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31">
+    </row>
+    <row r="38" spans="1:30">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5091,11 +4980,8 @@
       <c r="Z38">
         <v>7295</v>
       </c>
-      <c r="AE38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31">
+    </row>
+    <row r="39" spans="1:30">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5174,11 +5060,8 @@
       <c r="Z39">
         <v>7895</v>
       </c>
-      <c r="AE39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31">
+    </row>
+    <row r="40" spans="1:30">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5257,11 +5140,8 @@
       <c r="Z40">
         <v>9095</v>
       </c>
-      <c r="AE40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31">
+    </row>
+    <row r="41" spans="1:30">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5352,11 +5232,8 @@
       <c r="AD41">
         <v>0</v>
       </c>
-      <c r="AE41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31">
+    </row>
+    <row r="42" spans="1:30">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5435,11 +5312,8 @@
       <c r="Z42">
         <v>10295</v>
       </c>
-      <c r="AE42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:31">
+    </row>
+    <row r="43" spans="1:30">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5518,11 +5392,8 @@
       <c r="Z43">
         <v>12945</v>
       </c>
-      <c r="AE43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:31">
+    </row>
+    <row r="44" spans="1:30">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5613,11 +5484,8 @@
       <c r="AD44">
         <v>14417</v>
       </c>
-      <c r="AE44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31">
+    </row>
+    <row r="45" spans="1:30">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5708,11 +5576,8 @@
       <c r="AD45">
         <v>0</v>
       </c>
-      <c r="AE45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31">
+    </row>
+    <row r="46" spans="1:30">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5803,11 +5668,8 @@
       <c r="AD46">
         <v>0</v>
       </c>
-      <c r="AE46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:31">
+    </row>
+    <row r="47" spans="1:30">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5898,11 +5760,8 @@
       <c r="AD47">
         <v>0</v>
       </c>
-      <c r="AE47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31">
+    </row>
+    <row r="48" spans="1:30">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5993,11 +5852,8 @@
       <c r="AD48">
         <v>0</v>
       </c>
-      <c r="AE48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31">
+    </row>
+    <row r="49" spans="1:30">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6088,11 +5944,8 @@
       <c r="AD49">
         <v>24</v>
       </c>
-      <c r="AE49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31">
+    </row>
+    <row r="50" spans="1:30">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6183,11 +6036,8 @@
       <c r="AD50">
         <v>1194</v>
       </c>
-      <c r="AE50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:31">
+    </row>
+    <row r="51" spans="1:30">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6278,11 +6128,8 @@
       <c r="AD51">
         <v>0</v>
       </c>
-      <c r="AE51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31">
+    </row>
+    <row r="52" spans="1:30">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6373,11 +6220,8 @@
       <c r="AD52">
         <v>12680</v>
       </c>
-      <c r="AE52" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31">
+    </row>
+    <row r="53" spans="1:30">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6468,11 +6312,8 @@
       <c r="AD53">
         <v>0</v>
       </c>
-      <c r="AE53" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31">
+    </row>
+    <row r="54" spans="1:30">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6563,11 +6404,8 @@
       <c r="AD54">
         <v>0</v>
       </c>
-      <c r="AE54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:31">
+    </row>
+    <row r="55" spans="1:30">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6658,11 +6496,8 @@
       <c r="AD55">
         <v>19383</v>
       </c>
-      <c r="AE55" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:31">
+    </row>
+    <row r="56" spans="1:30">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6753,11 +6588,8 @@
       <c r="AD56">
         <v>0</v>
       </c>
-      <c r="AE56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31">
+    </row>
+    <row r="57" spans="1:30">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6848,11 +6680,8 @@
       <c r="AD57">
         <v>0</v>
       </c>
-      <c r="AE57" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31">
+    </row>
+    <row r="58" spans="1:30">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6931,11 +6760,8 @@
       <c r="Z58">
         <v>11845</v>
       </c>
-      <c r="AE58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31">
+    </row>
+    <row r="59" spans="1:30">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7026,11 +6852,8 @@
       <c r="AD59">
         <v>0</v>
       </c>
-      <c r="AE59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31">
+    </row>
+    <row r="60" spans="1:30">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7121,11 +6944,8 @@
       <c r="AD60">
         <v>0</v>
       </c>
-      <c r="AE60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:31">
+    </row>
+    <row r="61" spans="1:30">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7216,11 +7036,8 @@
       <c r="AD61">
         <v>0</v>
       </c>
-      <c r="AE61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:31">
+    </row>
+    <row r="62" spans="1:30">
       <c r="A62">
         <v>61</v>
       </c>
@@ -7299,11 +7116,8 @@
       <c r="Z62">
         <v>8495</v>
       </c>
-      <c r="AE62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:31">
+    </row>
+    <row r="63" spans="1:30">
       <c r="A63">
         <v>62</v>
       </c>
@@ -7382,11 +7196,8 @@
       <c r="Z63">
         <v>10595</v>
       </c>
-      <c r="AE63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:31">
+    </row>
+    <row r="64" spans="1:30">
       <c r="A64">
         <v>63</v>
       </c>
@@ -7477,11 +7288,8 @@
       <c r="AD64">
         <v>19383</v>
       </c>
-      <c r="AE64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:31">
+    </row>
+    <row r="65" spans="1:30">
       <c r="A65">
         <v>64</v>
       </c>
@@ -7572,11 +7380,8 @@
       <c r="AD65">
         <v>0</v>
       </c>
-      <c r="AE65" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:31">
+    </row>
+    <row r="66" spans="1:30">
       <c r="A66">
         <v>65</v>
       </c>
@@ -7667,11 +7472,8 @@
       <c r="AD66">
         <v>0</v>
       </c>
-      <c r="AE66" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:31">
+    </row>
+    <row r="67" spans="1:30">
       <c r="A67">
         <v>66</v>
       </c>
@@ -7750,11 +7552,8 @@
       <c r="Z67">
         <v>18280</v>
       </c>
-      <c r="AE67" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:31">
+    </row>
+    <row r="68" spans="1:30">
       <c r="A68">
         <v>67</v>
       </c>
@@ -7845,11 +7644,8 @@
       <c r="AD68">
         <v>0</v>
       </c>
-      <c r="AE68" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="69" spans="1:31">
+    </row>
+    <row r="69" spans="1:30">
       <c r="A69">
         <v>68</v>
       </c>
@@ -7940,11 +7736,8 @@
       <c r="AD69">
         <v>0</v>
       </c>
-      <c r="AE69" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="1:31">
+    </row>
+    <row r="70" spans="1:30">
       <c r="A70">
         <v>69</v>
       </c>
@@ -8035,11 +7828,8 @@
       <c r="AD70">
         <v>0</v>
       </c>
-      <c r="AE70" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="71" spans="1:31">
+    </row>
+    <row r="71" spans="1:30">
       <c r="A71">
         <v>70</v>
       </c>
@@ -8130,11 +7920,8 @@
       <c r="AD71">
         <v>0</v>
       </c>
-      <c r="AE71" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="72" spans="1:31">
+    </row>
+    <row r="72" spans="1:30">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8225,11 +8012,8 @@
       <c r="AD72">
         <v>0</v>
       </c>
-      <c r="AE72" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="1:31">
+    </row>
+    <row r="73" spans="1:30">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8308,11 +8092,8 @@
       <c r="Z73">
         <v>34184</v>
       </c>
-      <c r="AE73" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:31">
+    </row>
+    <row r="74" spans="1:30">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8391,11 +8172,8 @@
       <c r="Z74">
         <v>35056</v>
       </c>
-      <c r="AE74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:31">
+    </row>
+    <row r="75" spans="1:30">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8486,11 +8264,8 @@
       <c r="AD75">
         <v>0</v>
       </c>
-      <c r="AE75" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:31">
+    </row>
+    <row r="76" spans="1:30">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8581,11 +8356,8 @@
       <c r="AD76">
         <v>96605</v>
       </c>
-      <c r="AE76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:31">
+    </row>
+    <row r="77" spans="1:30">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8676,11 +8448,8 @@
       <c r="AD77">
         <v>0</v>
       </c>
-      <c r="AE77" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="78" spans="1:31">
+    </row>
+    <row r="78" spans="1:30">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8771,11 +8540,8 @@
       <c r="AD78">
         <v>22741</v>
       </c>
-      <c r="AE78" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="1:31">
+    </row>
+    <row r="79" spans="1:30">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8866,11 +8632,8 @@
       <c r="AD79">
         <v>0</v>
       </c>
-      <c r="AE79" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:31">
+    </row>
+    <row r="80" spans="1:30">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8961,11 +8724,8 @@
       <c r="AD80">
         <v>13897</v>
       </c>
-      <c r="AE80" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="81" spans="1:31">
+    </row>
+    <row r="81" spans="1:30">
       <c r="A81">
         <v>80</v>
       </c>
@@ -9056,11 +8816,8 @@
       <c r="AD81">
         <v>22741</v>
       </c>
-      <c r="AE81" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="82" spans="1:31">
+    </row>
+    <row r="82" spans="1:30">
       <c r="A82">
         <v>81</v>
       </c>
@@ -9151,11 +8908,8 @@
       <c r="AD82">
         <v>22741</v>
       </c>
-      <c r="AE82" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="83" spans="1:31">
+    </row>
+    <row r="83" spans="1:30">
       <c r="A83">
         <v>82</v>
       </c>
@@ -9246,11 +9000,8 @@
       <c r="AD83">
         <v>22741</v>
       </c>
-      <c r="AE83" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="84" spans="1:31">
+    </row>
+    <row r="84" spans="1:30">
       <c r="A84">
         <v>83</v>
       </c>
@@ -9341,11 +9092,8 @@
       <c r="AD84">
         <v>13897</v>
       </c>
-      <c r="AE84" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="85" spans="1:31">
+    </row>
+    <row r="85" spans="1:30">
       <c r="A85">
         <v>84</v>
       </c>
@@ -9436,11 +9184,8 @@
       <c r="AD85">
         <v>22741</v>
       </c>
-      <c r="AE85" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:31">
+    </row>
+    <row r="86" spans="1:30">
       <c r="A86">
         <v>85</v>
       </c>
@@ -9531,11 +9276,8 @@
       <c r="AD86">
         <v>22741</v>
       </c>
-      <c r="AE86" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:31">
+    </row>
+    <row r="87" spans="1:30">
       <c r="A87">
         <v>86</v>
       </c>
@@ -9626,11 +9368,8 @@
       <c r="AD87">
         <v>0</v>
       </c>
-      <c r="AE87" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="1:31">
+    </row>
+    <row r="88" spans="1:30">
       <c r="A88">
         <v>87</v>
       </c>
@@ -9721,11 +9460,8 @@
       <c r="AD88">
         <v>0</v>
       </c>
-      <c r="AE88" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="89" spans="1:31">
+    </row>
+    <row r="89" spans="1:30">
       <c r="A89">
         <v>88</v>
       </c>
@@ -9816,11 +9552,8 @@
       <c r="AD89">
         <v>13897</v>
       </c>
-      <c r="AE89" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="90" spans="1:31">
+    </row>
+    <row r="90" spans="1:30">
       <c r="A90">
         <v>89</v>
       </c>
@@ -9911,11 +9644,8 @@
       <c r="AD90">
         <v>22741</v>
       </c>
-      <c r="AE90" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:31">
+    </row>
+    <row r="91" spans="1:30">
       <c r="A91">
         <v>90</v>
       </c>
@@ -10006,11 +9736,8 @@
       <c r="AD91">
         <v>60913</v>
       </c>
-      <c r="AE91" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:31">
+    </row>
+    <row r="92" spans="1:30">
       <c r="A92">
         <v>91</v>
       </c>
@@ -10101,11 +9828,8 @@
       <c r="AD92">
         <v>227</v>
       </c>
-      <c r="AE92" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93" spans="1:31">
+    </row>
+    <row r="93" spans="1:30">
       <c r="A93">
         <v>92</v>
       </c>
@@ -10196,11 +9920,8 @@
       <c r="AD93">
         <v>285602</v>
       </c>
-      <c r="AE93" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="94" spans="1:31">
+    </row>
+    <row r="94" spans="1:30">
       <c r="A94">
         <v>93</v>
       </c>
@@ -10279,11 +10000,8 @@
       <c r="Z94">
         <v>6849</v>
       </c>
-      <c r="AE94" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="95" spans="1:31">
+    </row>
+    <row r="95" spans="1:30">
       <c r="A95">
         <v>94</v>
       </c>
@@ -10374,11 +10092,8 @@
       <c r="AD95">
         <v>27409</v>
       </c>
-      <c r="AE95" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="1:31">
+    </row>
+    <row r="96" spans="1:30">
       <c r="A96">
         <v>95</v>
       </c>
@@ -10469,11 +10184,8 @@
       <c r="AD96">
         <v>14239</v>
       </c>
-      <c r="AE96" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="97" spans="1:31">
+    </row>
+    <row r="97" spans="1:30">
       <c r="A97">
         <v>96</v>
       </c>
@@ -10564,11 +10276,8 @@
       <c r="AD97">
         <v>62535</v>
       </c>
-      <c r="AE97" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="98" spans="1:31">
+    </row>
+    <row r="98" spans="1:30">
       <c r="A98">
         <v>97</v>
       </c>
@@ -10647,11 +10356,8 @@
       <c r="Z98">
         <v>7499</v>
       </c>
-      <c r="AE98" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="99" spans="1:31">
+    </row>
+    <row r="99" spans="1:30">
       <c r="A99">
         <v>98</v>
       </c>
@@ -10742,11 +10448,8 @@
       <c r="AD99">
         <v>0</v>
       </c>
-      <c r="AE99" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="100" spans="1:31">
+    </row>
+    <row r="100" spans="1:30">
       <c r="A100">
         <v>99</v>
       </c>
@@ -10825,11 +10528,8 @@
       <c r="Z100">
         <v>8249</v>
       </c>
-      <c r="AE100" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="101" spans="1:31">
+    </row>
+    <row r="101" spans="1:30">
       <c r="A101">
         <v>100</v>
       </c>
@@ -10920,11 +10620,8 @@
       <c r="AD101">
         <v>285602</v>
       </c>
-      <c r="AE101" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="102" spans="1:31">
+    </row>
+    <row r="102" spans="1:30">
       <c r="A102">
         <v>101</v>
       </c>
@@ -11015,11 +10712,8 @@
       <c r="AD102">
         <v>1226</v>
       </c>
-      <c r="AE102" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="103" spans="1:31">
+    </row>
+    <row r="103" spans="1:30">
       <c r="A103">
         <v>102</v>
       </c>
@@ -11098,11 +10792,8 @@
       <c r="Z103">
         <v>13499</v>
       </c>
-      <c r="AE103" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="104" spans="1:31">
+    </row>
+    <row r="104" spans="1:30">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11181,11 +10872,8 @@
       <c r="Z104">
         <v>14399</v>
       </c>
-      <c r="AE104" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="105" spans="1:31">
+    </row>
+    <row r="105" spans="1:30">
       <c r="A105">
         <v>104</v>
       </c>
@@ -11276,11 +10964,8 @@
       <c r="AD105">
         <v>0</v>
       </c>
-      <c r="AE105" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="106" spans="1:31">
+    </row>
+    <row r="106" spans="1:30">
       <c r="A106">
         <v>105</v>
       </c>
@@ -11371,11 +11056,8 @@
       <c r="AD106">
         <v>162010</v>
       </c>
-      <c r="AE106" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="107" spans="1:31">
+    </row>
+    <row r="107" spans="1:30">
       <c r="A107">
         <v>106</v>
       </c>
@@ -11466,11 +11148,8 @@
       <c r="AD107">
         <v>82969</v>
       </c>
-      <c r="AE107" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="108" spans="1:31">
+    </row>
+    <row r="108" spans="1:30">
       <c r="A108">
         <v>107</v>
       </c>
@@ -11549,11 +11228,8 @@
       <c r="Z108">
         <v>18399</v>
       </c>
-      <c r="AE108" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="109" spans="1:31">
+    </row>
+    <row r="109" spans="1:30">
       <c r="A109">
         <v>108</v>
       </c>
@@ -11644,11 +11320,8 @@
       <c r="AD109">
         <v>0</v>
       </c>
-      <c r="AE109" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="110" spans="1:31">
+    </row>
+    <row r="110" spans="1:30">
       <c r="A110">
         <v>109</v>
       </c>
@@ -11739,11 +11412,8 @@
       <c r="AD110">
         <v>0</v>
       </c>
-      <c r="AE110" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="111" spans="1:31">
+    </row>
+    <row r="111" spans="1:30">
       <c r="A111">
         <v>110</v>
       </c>
@@ -11834,11 +11504,8 @@
       <c r="AD111">
         <v>0</v>
       </c>
-      <c r="AE111" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="112" spans="1:31">
+    </row>
+    <row r="112" spans="1:30">
       <c r="A112">
         <v>111</v>
       </c>
@@ -11929,11 +11596,8 @@
       <c r="AD112">
         <v>0</v>
       </c>
-      <c r="AE112" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="113" spans="1:31">
+    </row>
+    <row r="113" spans="1:30">
       <c r="A113">
         <v>112</v>
       </c>
@@ -12024,11 +11688,8 @@
       <c r="AD113">
         <v>0</v>
       </c>
-      <c r="AE113" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="114" spans="1:31">
+    </row>
+    <row r="114" spans="1:30">
       <c r="A114">
         <v>113</v>
       </c>
@@ -12119,11 +11780,8 @@
       <c r="AD114">
         <v>0</v>
       </c>
-      <c r="AE114" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="115" spans="1:31">
+    </row>
+    <row r="115" spans="1:30">
       <c r="A115">
         <v>114</v>
       </c>
@@ -12214,11 +11872,8 @@
       <c r="AD115">
         <v>0</v>
       </c>
-      <c r="AE115" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="116" spans="1:31">
+    </row>
+    <row r="116" spans="1:30">
       <c r="A116">
         <v>115</v>
       </c>
@@ -12309,11 +11964,8 @@
       <c r="AD116">
         <v>0</v>
       </c>
-      <c r="AE116" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="117" spans="1:31">
+    </row>
+    <row r="117" spans="1:30">
       <c r="A117">
         <v>116</v>
       </c>
@@ -12404,11 +12056,8 @@
       <c r="AD117">
         <v>0</v>
       </c>
-      <c r="AE117" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="118" spans="1:31">
+    </row>
+    <row r="118" spans="1:30">
       <c r="A118">
         <v>117</v>
       </c>
@@ -12499,11 +12148,8 @@
       <c r="AD118">
         <v>0</v>
       </c>
-      <c r="AE118" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="119" spans="1:31">
+    </row>
+    <row r="119" spans="1:30">
       <c r="A119">
         <v>118</v>
       </c>
@@ -12594,11 +12240,8 @@
       <c r="AD119">
         <v>0</v>
       </c>
-      <c r="AE119" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="120" spans="1:31">
+    </row>
+    <row r="120" spans="1:30">
       <c r="A120">
         <v>119</v>
       </c>
@@ -12689,11 +12332,8 @@
       <c r="AD120">
         <v>0</v>
       </c>
-      <c r="AE120" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="121" spans="1:31">
+    </row>
+    <row r="121" spans="1:30">
       <c r="A121">
         <v>120</v>
       </c>
@@ -12784,11 +12424,8 @@
       <c r="AD121">
         <v>0</v>
       </c>
-      <c r="AE121" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="122" spans="1:31">
+    </row>
+    <row r="122" spans="1:30">
       <c r="A122">
         <v>121</v>
       </c>
@@ -12879,11 +12516,8 @@
       <c r="AD122">
         <v>0</v>
       </c>
-      <c r="AE122" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="123" spans="1:31">
+    </row>
+    <row r="123" spans="1:30">
       <c r="A123">
         <v>122</v>
       </c>
@@ -12974,11 +12608,8 @@
       <c r="AD123">
         <v>0</v>
       </c>
-      <c r="AE123" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="124" spans="1:31">
+    </row>
+    <row r="124" spans="1:30">
       <c r="A124">
         <v>123</v>
       </c>
@@ -13069,11 +12700,8 @@
       <c r="AD124">
         <v>0</v>
       </c>
-      <c r="AE124" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="125" spans="1:31">
+    </row>
+    <row r="125" spans="1:30">
       <c r="A125">
         <v>124</v>
       </c>
@@ -13164,11 +12792,8 @@
       <c r="AD125">
         <v>0</v>
       </c>
-      <c r="AE125" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="126" spans="1:31">
+    </row>
+    <row r="126" spans="1:30">
       <c r="A126">
         <v>125</v>
       </c>
@@ -13259,11 +12884,8 @@
       <c r="AD126">
         <v>0</v>
       </c>
-      <c r="AE126" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="127" spans="1:31">
+    </row>
+    <row r="127" spans="1:30">
       <c r="A127">
         <v>126</v>
       </c>
@@ -13354,11 +12976,8 @@
       <c r="AD127">
         <v>15756</v>
       </c>
-      <c r="AE127" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="128" spans="1:31">
+    </row>
+    <row r="128" spans="1:30">
       <c r="A128">
         <v>127</v>
       </c>
@@ -13449,11 +13068,8 @@
       <c r="AD128">
         <v>5097</v>
       </c>
-      <c r="AE128" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="129" spans="1:31">
+    </row>
+    <row r="129" spans="1:30">
       <c r="A129">
         <v>128</v>
       </c>
@@ -13544,11 +13160,8 @@
       <c r="AD129">
         <v>16310</v>
       </c>
-      <c r="AE129" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="130" spans="1:31">
+    </row>
+    <row r="130" spans="1:30">
       <c r="A130">
         <v>129</v>
       </c>
@@ -13639,11 +13252,8 @@
       <c r="AD130">
         <v>0</v>
       </c>
-      <c r="AE130" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="131" spans="1:31">
+    </row>
+    <row r="131" spans="1:30">
       <c r="A131">
         <v>130</v>
       </c>
@@ -13734,11 +13344,8 @@
       <c r="AD131">
         <v>16310</v>
       </c>
-      <c r="AE131" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="132" spans="1:31">
+    </row>
+    <row r="132" spans="1:30">
       <c r="A132">
         <v>131</v>
       </c>
@@ -13817,11 +13424,8 @@
       <c r="Z132">
         <v>9295</v>
       </c>
-      <c r="AE132" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="133" spans="1:31">
+    </row>
+    <row r="133" spans="1:30">
       <c r="A133">
         <v>132</v>
       </c>
@@ -13912,11 +13516,8 @@
       <c r="AD133">
         <v>0</v>
       </c>
-      <c r="AE133" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="134" spans="1:31">
+    </row>
+    <row r="134" spans="1:30">
       <c r="A134">
         <v>133</v>
       </c>
@@ -14007,11 +13608,8 @@
       <c r="AD134">
         <v>0</v>
       </c>
-      <c r="AE134" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="135" spans="1:31">
+    </row>
+    <row r="135" spans="1:30">
       <c r="A135">
         <v>134</v>
       </c>
@@ -14102,11 +13700,8 @@
       <c r="AD135">
         <v>0</v>
       </c>
-      <c r="AE135" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="136" spans="1:31">
+    </row>
+    <row r="136" spans="1:30">
       <c r="A136">
         <v>135</v>
       </c>
@@ -14197,11 +13792,8 @@
       <c r="AD136">
         <v>0</v>
       </c>
-      <c r="AE136" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="137" spans="1:31">
+    </row>
+    <row r="137" spans="1:30">
       <c r="A137">
         <v>136</v>
       </c>
@@ -14292,11 +13884,8 @@
       <c r="AD137">
         <v>0</v>
       </c>
-      <c r="AE137" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="138" spans="1:31">
+    </row>
+    <row r="138" spans="1:30">
       <c r="A138">
         <v>137</v>
       </c>
@@ -14387,11 +13976,8 @@
       <c r="AD138">
         <v>0</v>
       </c>
-      <c r="AE138" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="139" spans="1:31">
+    </row>
+    <row r="139" spans="1:30">
       <c r="A139">
         <v>138</v>
       </c>
@@ -14482,11 +14068,8 @@
       <c r="AD139">
         <v>0</v>
       </c>
-      <c r="AE139" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="140" spans="1:31">
+    </row>
+    <row r="140" spans="1:30">
       <c r="A140">
         <v>139</v>
       </c>
@@ -14577,11 +14160,8 @@
       <c r="AD140">
         <v>2320</v>
       </c>
-      <c r="AE140" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="141" spans="1:31">
+    </row>
+    <row r="141" spans="1:30">
       <c r="A141">
         <v>140</v>
       </c>
@@ -14672,11 +14252,8 @@
       <c r="AD141">
         <v>1002</v>
       </c>
-      <c r="AE141" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="142" spans="1:31">
+    </row>
+    <row r="142" spans="1:30">
       <c r="A142">
         <v>141</v>
       </c>
@@ -14767,11 +14344,8 @@
       <c r="AD142">
         <v>3423</v>
       </c>
-      <c r="AE142" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="143" spans="1:31">
+    </row>
+    <row r="143" spans="1:30">
       <c r="A143">
         <v>142</v>
       </c>
@@ -14862,11 +14436,8 @@
       <c r="AD143">
         <v>1213</v>
       </c>
-      <c r="AE143" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="144" spans="1:31">
+    </row>
+    <row r="144" spans="1:30">
       <c r="A144">
         <v>143</v>
       </c>
@@ -14957,11 +14528,8 @@
       <c r="AD144">
         <v>2320</v>
       </c>
-      <c r="AE144" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="145" spans="1:31">
+    </row>
+    <row r="145" spans="1:30">
       <c r="A145">
         <v>144</v>
       </c>
@@ -15052,11 +14620,8 @@
       <c r="AD145">
         <v>0</v>
       </c>
-      <c r="AE145" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="146" spans="1:31">
+    </row>
+    <row r="146" spans="1:30">
       <c r="A146">
         <v>145</v>
       </c>
@@ -15147,11 +14712,8 @@
       <c r="AD146">
         <v>0</v>
       </c>
-      <c r="AE146" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="147" spans="1:31">
+    </row>
+    <row r="147" spans="1:30">
       <c r="A147">
         <v>146</v>
       </c>
@@ -15242,11 +14804,8 @@
       <c r="AD147">
         <v>0</v>
       </c>
-      <c r="AE147" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="148" spans="1:31">
+    </row>
+    <row r="148" spans="1:30">
       <c r="A148">
         <v>147</v>
       </c>
@@ -15337,11 +14896,8 @@
       <c r="AD148">
         <v>0</v>
       </c>
-      <c r="AE148" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="149" spans="1:31">
+    </row>
+    <row r="149" spans="1:30">
       <c r="A149">
         <v>148</v>
       </c>
@@ -15432,11 +14988,8 @@
       <c r="AD149">
         <v>0</v>
       </c>
-      <c r="AE149" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="150" spans="1:31">
+    </row>
+    <row r="150" spans="1:30">
       <c r="A150">
         <v>149</v>
       </c>
@@ -15527,11 +15080,8 @@
       <c r="AD150">
         <v>2320</v>
       </c>
-      <c r="AE150" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="151" spans="1:31">
+    </row>
+    <row r="151" spans="1:30">
       <c r="A151">
         <v>150</v>
       </c>
@@ -15622,11 +15172,8 @@
       <c r="AD151">
         <v>2320</v>
       </c>
-      <c r="AE151" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="152" spans="1:31">
+    </row>
+    <row r="152" spans="1:30">
       <c r="A152">
         <v>151</v>
       </c>
@@ -15717,11 +15264,8 @@
       <c r="AD152">
         <v>0</v>
       </c>
-      <c r="AE152" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="153" spans="1:31">
+    </row>
+    <row r="153" spans="1:30">
       <c r="A153">
         <v>152</v>
       </c>
@@ -15812,11 +15356,8 @@
       <c r="AD153">
         <v>0</v>
       </c>
-      <c r="AE153" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="154" spans="1:31">
+    </row>
+    <row r="154" spans="1:30">
       <c r="A154">
         <v>153</v>
       </c>
@@ -15907,11 +15448,8 @@
       <c r="AD154">
         <v>142720</v>
       </c>
-      <c r="AE154" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="155" spans="1:31">
+    </row>
+    <row r="155" spans="1:30">
       <c r="A155">
         <v>154</v>
       </c>
@@ -16002,11 +15540,8 @@
       <c r="AD155">
         <v>0</v>
       </c>
-      <c r="AE155" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="156" spans="1:31">
+    </row>
+    <row r="156" spans="1:30">
       <c r="A156">
         <v>155</v>
       </c>
@@ -16097,11 +15632,8 @@
       <c r="AD156">
         <v>248993</v>
       </c>
-      <c r="AE156" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="157" spans="1:31">
+    </row>
+    <row r="157" spans="1:30">
       <c r="A157">
         <v>156</v>
       </c>
@@ -16192,11 +15724,8 @@
       <c r="AD157">
         <v>0</v>
       </c>
-      <c r="AE157" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="158" spans="1:31">
+    </row>
+    <row r="158" spans="1:30">
       <c r="A158">
         <v>157</v>
       </c>
@@ -16287,11 +15816,8 @@
       <c r="AD158">
         <v>0</v>
       </c>
-      <c r="AE158" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="159" spans="1:31">
+    </row>
+    <row r="159" spans="1:30">
       <c r="A159">
         <v>158</v>
       </c>
@@ -16382,11 +15908,8 @@
       <c r="AD159">
         <v>142720</v>
       </c>
-      <c r="AE159" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="160" spans="1:31">
+    </row>
+    <row r="160" spans="1:30">
       <c r="A160">
         <v>159</v>
       </c>
@@ -16477,11 +16000,8 @@
       <c r="AD160">
         <v>0</v>
       </c>
-      <c r="AE160" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="161" spans="1:31">
+    </row>
+    <row r="161" spans="1:30">
       <c r="A161">
         <v>160</v>
       </c>
@@ -16572,11 +16092,8 @@
       <c r="AD161">
         <v>142720</v>
       </c>
-      <c r="AE161" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="162" spans="1:31">
+    </row>
+    <row r="162" spans="1:30">
       <c r="A162">
         <v>161</v>
       </c>
@@ -16667,11 +16184,8 @@
       <c r="AD162">
         <v>0</v>
       </c>
-      <c r="AE162" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="163" spans="1:31">
+    </row>
+    <row r="163" spans="1:30">
       <c r="A163">
         <v>162</v>
       </c>
@@ -16762,11 +16276,8 @@
       <c r="AD163">
         <v>142720</v>
       </c>
-      <c r="AE163" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="164" spans="1:31">
+    </row>
+    <row r="164" spans="1:30">
       <c r="A164">
         <v>163</v>
       </c>
@@ -16857,11 +16368,8 @@
       <c r="AD164">
         <v>0</v>
       </c>
-      <c r="AE164" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="165" spans="1:31">
+    </row>
+    <row r="165" spans="1:30">
       <c r="A165">
         <v>164</v>
       </c>
@@ -16952,11 +16460,8 @@
       <c r="AD165">
         <v>142720</v>
       </c>
-      <c r="AE165" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="166" spans="1:31">
+    </row>
+    <row r="166" spans="1:30">
       <c r="A166">
         <v>165</v>
       </c>
@@ -17047,11 +16552,8 @@
       <c r="AD166">
         <v>0</v>
       </c>
-      <c r="AE166" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="167" spans="1:31">
+    </row>
+    <row r="167" spans="1:30">
       <c r="A167">
         <v>166</v>
       </c>
@@ -17142,11 +16644,8 @@
       <c r="AD167">
         <v>0</v>
       </c>
-      <c r="AE167" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="168" spans="1:31">
+    </row>
+    <row r="168" spans="1:30">
       <c r="A168">
         <v>167</v>
       </c>
@@ -17237,11 +16736,8 @@
       <c r="AD168">
         <v>0</v>
       </c>
-      <c r="AE168" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="169" spans="1:31">
+    </row>
+    <row r="169" spans="1:30">
       <c r="A169">
         <v>168</v>
       </c>
@@ -17332,11 +16828,8 @@
       <c r="AD169">
         <v>0</v>
       </c>
-      <c r="AE169" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="170" spans="1:31">
+    </row>
+    <row r="170" spans="1:30">
       <c r="A170">
         <v>169</v>
       </c>
@@ -17427,11 +16920,8 @@
       <c r="AD170">
         <v>142720</v>
       </c>
-      <c r="AE170" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="171" spans="1:31">
+    </row>
+    <row r="171" spans="1:30">
       <c r="A171">
         <v>170</v>
       </c>
@@ -17522,11 +17012,8 @@
       <c r="AD171">
         <v>0</v>
       </c>
-      <c r="AE171" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="172" spans="1:31">
+    </row>
+    <row r="172" spans="1:30">
       <c r="A172">
         <v>171</v>
       </c>
@@ -17617,11 +17104,8 @@
       <c r="AD172">
         <v>0</v>
       </c>
-      <c r="AE172" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="173" spans="1:31">
+    </row>
+    <row r="173" spans="1:30">
       <c r="A173">
         <v>172</v>
       </c>
@@ -17712,11 +17196,8 @@
       <c r="AD173">
         <v>142720</v>
       </c>
-      <c r="AE173" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="174" spans="1:31">
+    </row>
+    <row r="174" spans="1:30">
       <c r="A174">
         <v>173</v>
       </c>
@@ -17807,11 +17288,8 @@
       <c r="AD174">
         <v>0</v>
       </c>
-      <c r="AE174" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="175" spans="1:31">
+    </row>
+    <row r="175" spans="1:30">
       <c r="A175">
         <v>174</v>
       </c>
@@ -17902,11 +17380,8 @@
       <c r="AD175">
         <v>142720</v>
       </c>
-      <c r="AE175" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="176" spans="1:31">
+    </row>
+    <row r="176" spans="1:30">
       <c r="A176">
         <v>175</v>
       </c>
@@ -17997,11 +17472,8 @@
       <c r="AD176">
         <v>0</v>
       </c>
-      <c r="AE176" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="177" spans="1:31">
+    </row>
+    <row r="177" spans="1:30">
       <c r="A177">
         <v>176</v>
       </c>
@@ -18092,11 +17564,8 @@
       <c r="AD177">
         <v>0</v>
       </c>
-      <c r="AE177" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="178" spans="1:31">
+    </row>
+    <row r="178" spans="1:30">
       <c r="A178">
         <v>177</v>
       </c>
@@ -18187,11 +17656,8 @@
       <c r="AD178">
         <v>142720</v>
       </c>
-      <c r="AE178" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="179" spans="1:31">
+    </row>
+    <row r="179" spans="1:30">
       <c r="A179">
         <v>178</v>
       </c>
@@ -18282,11 +17748,8 @@
       <c r="AD179">
         <v>0</v>
       </c>
-      <c r="AE179" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="180" spans="1:31">
+    </row>
+    <row r="180" spans="1:30">
       <c r="A180">
         <v>179</v>
       </c>
@@ -18377,11 +17840,8 @@
       <c r="AD180">
         <v>142720</v>
       </c>
-      <c r="AE180" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="181" spans="1:31">
+    </row>
+    <row r="181" spans="1:30">
       <c r="A181">
         <v>180</v>
       </c>
@@ -18472,11 +17932,8 @@
       <c r="AD181">
         <v>0</v>
       </c>
-      <c r="AE181" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="182" spans="1:31">
+    </row>
+    <row r="182" spans="1:30">
       <c r="A182">
         <v>181</v>
       </c>
@@ -18567,11 +18024,8 @@
       <c r="AD182">
         <v>0</v>
       </c>
-      <c r="AE182" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="183" spans="1:31">
+    </row>
+    <row r="183" spans="1:30">
       <c r="A183">
         <v>182</v>
       </c>
@@ -18662,11 +18116,8 @@
       <c r="AD183">
         <v>0</v>
       </c>
-      <c r="AE183" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="184" spans="1:31">
+    </row>
+    <row r="184" spans="1:30">
       <c r="A184">
         <v>183</v>
       </c>
@@ -18757,11 +18208,8 @@
       <c r="AD184">
         <v>0</v>
       </c>
-      <c r="AE184" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="185" spans="1:31">
+    </row>
+    <row r="185" spans="1:30">
       <c r="A185">
         <v>184</v>
       </c>
@@ -18852,11 +18300,8 @@
       <c r="AD185">
         <v>0</v>
       </c>
-      <c r="AE185" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="186" spans="1:31">
+    </row>
+    <row r="186" spans="1:30">
       <c r="A186">
         <v>185</v>
       </c>
@@ -18947,11 +18392,8 @@
       <c r="AD186">
         <v>0</v>
       </c>
-      <c r="AE186" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="187" spans="1:31">
+    </row>
+    <row r="187" spans="1:30">
       <c r="A187">
         <v>186</v>
       </c>
@@ -19042,11 +18484,8 @@
       <c r="AD187">
         <v>0</v>
       </c>
-      <c r="AE187" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="188" spans="1:31">
+    </row>
+    <row r="188" spans="1:30">
       <c r="A188">
         <v>187</v>
       </c>
@@ -19137,11 +18576,8 @@
       <c r="AD188">
         <v>0</v>
       </c>
-      <c r="AE188" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="189" spans="1:31">
+    </row>
+    <row r="189" spans="1:30">
       <c r="A189">
         <v>188</v>
       </c>
@@ -19232,11 +18668,8 @@
       <c r="AD189">
         <v>0</v>
       </c>
-      <c r="AE189" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="190" spans="1:31">
+    </row>
+    <row r="190" spans="1:30">
       <c r="A190">
         <v>189</v>
       </c>
@@ -19327,11 +18760,8 @@
       <c r="AD190">
         <v>0</v>
       </c>
-      <c r="AE190" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="191" spans="1:31">
+    </row>
+    <row r="191" spans="1:30">
       <c r="A191">
         <v>190</v>
       </c>
@@ -19422,11 +18852,8 @@
       <c r="AD191">
         <v>0</v>
       </c>
-      <c r="AE191" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="192" spans="1:31">
+    </row>
+    <row r="192" spans="1:30">
       <c r="A192">
         <v>191</v>
       </c>
@@ -19517,11 +18944,8 @@
       <c r="AD192">
         <v>0</v>
       </c>
-      <c r="AE192" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="193" spans="1:31">
+    </row>
+    <row r="193" spans="1:30">
       <c r="A193">
         <v>192</v>
       </c>
@@ -19612,11 +19036,8 @@
       <c r="AD193">
         <v>0</v>
       </c>
-      <c r="AE193" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="194" spans="1:31">
+    </row>
+    <row r="194" spans="1:30">
       <c r="A194">
         <v>193</v>
       </c>
@@ -19707,11 +19128,8 @@
       <c r="AD194">
         <v>0</v>
       </c>
-      <c r="AE194" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="195" spans="1:31">
+    </row>
+    <row r="195" spans="1:30">
       <c r="A195">
         <v>194</v>
       </c>
@@ -19802,11 +19220,8 @@
       <c r="AD195">
         <v>0</v>
       </c>
-      <c r="AE195" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="196" spans="1:31">
+    </row>
+    <row r="196" spans="1:30">
       <c r="A196">
         <v>195</v>
       </c>
@@ -19897,11 +19312,8 @@
       <c r="AD196">
         <v>0</v>
       </c>
-      <c r="AE196" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="197" spans="1:31">
+    </row>
+    <row r="197" spans="1:30">
       <c r="A197">
         <v>196</v>
       </c>
@@ -19992,11 +19404,8 @@
       <c r="AD197">
         <v>0</v>
       </c>
-      <c r="AE197" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="198" spans="1:31">
+    </row>
+    <row r="198" spans="1:30">
       <c r="A198">
         <v>197</v>
       </c>
@@ -20087,11 +19496,8 @@
       <c r="AD198">
         <v>0</v>
       </c>
-      <c r="AE198" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="199" spans="1:31">
+    </row>
+    <row r="199" spans="1:30">
       <c r="A199">
         <v>198</v>
       </c>
@@ -20182,11 +19588,8 @@
       <c r="AD199">
         <v>0</v>
       </c>
-      <c r="AE199" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="200" spans="1:31">
+    </row>
+    <row r="200" spans="1:30">
       <c r="A200">
         <v>199</v>
       </c>
@@ -20277,11 +19680,8 @@
       <c r="AD200">
         <v>0</v>
       </c>
-      <c r="AE200" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="201" spans="1:31">
+    </row>
+    <row r="201" spans="1:30">
       <c r="A201">
         <v>200</v>
       </c>
@@ -20372,11 +19772,8 @@
       <c r="AD201">
         <v>0</v>
       </c>
-      <c r="AE201" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="202" spans="1:31">
+    </row>
+    <row r="202" spans="1:30">
       <c r="A202">
         <v>201</v>
       </c>
@@ -20467,11 +19864,8 @@
       <c r="AD202">
         <v>0</v>
       </c>
-      <c r="AE202" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="203" spans="1:31">
+    </row>
+    <row r="203" spans="1:30">
       <c r="A203">
         <v>202</v>
       </c>
@@ -20562,11 +19956,8 @@
       <c r="AD203">
         <v>0</v>
       </c>
-      <c r="AE203" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="204" spans="1:31">
+    </row>
+    <row r="204" spans="1:30">
       <c r="A204">
         <v>203</v>
       </c>
@@ -20657,11 +20048,8 @@
       <c r="AD204">
         <v>0</v>
       </c>
-      <c r="AE204" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="205" spans="1:31">
+    </row>
+    <row r="205" spans="1:30">
       <c r="A205">
         <v>204</v>
       </c>
@@ -20752,11 +20140,8 @@
       <c r="AD205">
         <v>0</v>
       </c>
-      <c r="AE205" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="206" spans="1:31">
+    </row>
+    <row r="206" spans="1:30">
       <c r="A206">
         <v>205</v>
       </c>
@@ -20846,9 +20231,6 @@
       </c>
       <c r="AD206">
         <v>0</v>
-      </c>
-      <c r="AE206" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>